<commit_message>
gnome-multi-writer added for Debian
</commit_message>
<xml_diff>
--- a/Sources/install/Support Database.xlsx
+++ b/Sources/install/Support Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">Program</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">wamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gnome-multi-writer</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+      <selection pane="topLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -818,6 +821,14 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="3"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>